<commit_message>
Se agrego menu popup a la tabla
se agrego menu de PopUp a la tabla con opciones de agregar,modificar y eliminar datos a la ventana de consulta de articulos
</commit_message>
<xml_diff>
--- a/SINF/src/datos/current/Articulos.xlsx
+++ b/SINF/src/datos/current/Articulos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="148">
   <si>
     <t>ARTICULOS</t>
   </si>
@@ -68,12 +68,6 @@
     <t>Que los remolques y análogos no cumplan con las debidas condiciones de seguridad.</t>
   </si>
   <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>Circulación del vehículo en zona prohibid con exeso de dimensiones o fuera de horarios permitidos.</t>
-  </si>
-  <si>
     <t>23, fracción I, c)</t>
   </si>
   <si>
@@ -89,12 +83,6 @@
     <t>Multa de 20 UMA.</t>
   </si>
   <si>
-    <t>23, fracción I, e) y f)</t>
-  </si>
-  <si>
-    <t>Usar placas con cualquier alteración que impidan su legibilidad.</t>
-  </si>
-  <si>
     <t>23, fracción I, g)</t>
   </si>
   <si>
@@ -104,48 +92,18 @@
     <t>23, fracción II</t>
   </si>
   <si>
-    <t>Que los vehículos no se encuentren en condiciones adecudas para su funcionamiento.</t>
-  </si>
-  <si>
-    <t>Multa de 10 UMA y suspensión de drecho de tránsito y transporte hasta por 90 dias.</t>
-  </si>
-  <si>
-    <t>23, fracción III</t>
-  </si>
-  <si>
-    <t>Falta de claxon.</t>
+    <t>Vehiculo que no se encuentre en buen estado de funcionamiento para que su uso se realice en aceptables condiciones de seguridad.</t>
   </si>
   <si>
     <t>Multa de 3 UMA.</t>
   </si>
   <si>
-    <t>Vehiculo que no se encuentre en buen estado de funcionamiento para que su uso se realice en aceptables condiciones de seguridad.</t>
-  </si>
-  <si>
-    <t>23, fracción XVII</t>
-  </si>
-  <si>
-    <t>Portación de calocmanias en el vehículo que hagan apologia de un delito.</t>
-  </si>
-  <si>
     <t>23, fracción XV</t>
   </si>
   <si>
     <t>Circulación de vehiculo cristalizado o cubiertas de pintura o materiales refleantes los cuales tengan una transparencia de al menos 75%.</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>Que las motocicletas no se encuentren en adecuadas condiciones.</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>Que las bicicletas o bicimotos no se encuentren en condiciones óptimas.</t>
-  </si>
-  <si>
     <t>32, fracción I</t>
   </si>
   <si>
@@ -303,12 +261,6 @@
   </si>
   <si>
     <t>Obstruir la circulacion en un crucero.</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>Circular violando las reglas en intersección no controladas por semáforos o policias de vialidad.</t>
   </si>
   <si>
     <t>55</t>
@@ -650,18 +602,18 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -672,106 +624,106 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -782,7 +734,7 @@
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -793,26 +745,26 @@
         <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
@@ -820,43 +772,43 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
         <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
         <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
@@ -864,24 +816,24 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
@@ -892,7 +844,7 @@
         <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32">
@@ -903,59 +855,59 @@
         <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
@@ -963,46 +915,46 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42">
@@ -1013,7 +965,7 @@
         <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
@@ -1024,7 +976,7 @@
         <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44">
@@ -1046,7 +998,7 @@
         <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46">
@@ -1057,7 +1009,7 @@
         <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47">
@@ -1068,7 +1020,7 @@
         <v>102</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48">
@@ -1112,7 +1064,7 @@
         <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52">
@@ -1134,7 +1086,7 @@
         <v>114</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54">
@@ -1145,26 +1097,26 @@
         <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
         <v>117</v>
       </c>
-      <c r="B55" t="s">
-        <v>118</v>
-      </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
         <v>119</v>
-      </c>
-      <c r="B56" t="s">
-        <v>120</v>
       </c>
       <c r="C56" t="s">
         <v>10</v>
@@ -1172,10 +1124,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" t="s">
         <v>121</v>
-      </c>
-      <c r="B57" t="s">
-        <v>122</v>
       </c>
       <c r="C57" t="s">
         <v>10</v>
@@ -1183,68 +1135,68 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" t="s">
         <v>123</v>
       </c>
-      <c r="B58" t="s">
-        <v>124</v>
-      </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" t="s">
         <v>125</v>
       </c>
-      <c r="B59" t="s">
-        <v>126</v>
-      </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" t="s">
         <v>127</v>
       </c>
-      <c r="B60" t="s">
-        <v>128</v>
-      </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" t="s">
         <v>129</v>
       </c>
-      <c r="B61" t="s">
-        <v>130</v>
-      </c>
       <c r="C61" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" t="s">
         <v>131</v>
       </c>
-      <c r="B62" t="s">
-        <v>132</v>
-      </c>
       <c r="C62" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" t="s">
         <v>133</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64">
@@ -1266,139 +1218,51 @@
         <v>137</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C66" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>146</v>
-      </c>
-      <c r="B70" t="s">
-        <v>147</v>
-      </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>148</v>
-      </c>
-      <c r="B71" t="s">
-        <v>149</v>
-      </c>
-      <c r="C71" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>150</v>
-      </c>
-      <c r="B72" t="s">
-        <v>151</v>
-      </c>
-      <c r="C72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>152</v>
-      </c>
-      <c r="B73" t="s">
-        <v>153</v>
-      </c>
-      <c r="C73" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>155</v>
-      </c>
-      <c r="B74" t="s">
-        <v>156</v>
-      </c>
-      <c r="C74" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>158</v>
-      </c>
-      <c r="B75" t="s">
-        <v>159</v>
-      </c>
-      <c r="C75" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>160</v>
-      </c>
-      <c r="B76" t="s">
-        <v>161</v>
-      </c>
-      <c r="C76" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>162</v>
-      </c>
-      <c r="B77" t="s">
-        <v>163</v>
-      </c>
-      <c r="C77" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>